<commit_message>
testing upcorse and delete functional
</commit_message>
<xml_diff>
--- a/eth_journal/root_Hours_Plan.xlsx
+++ b/eth_journal/root_Hours_Plan.xlsx
@@ -31,7 +31,7 @@
     <t>Русский язык</t>
   </si>
   <si>
-    <t>2024ab</t>
+    <t>31ab</t>
   </si>
   <si>
     <t>Биология</t>
@@ -40,7 +40,7 @@
     <t>Предмет_1</t>
   </si>
   <si>
-    <t>2024аа</t>
+    <t>21аа</t>
   </si>
 </sst>
 </file>

</xml_diff>